<commit_message>
Changed default IP of Network tables client to the rRIO's IP
We successfully tested the regular NTC on the robot.
</commit_message>
<xml_diff>
--- a/SlideWinder/Robot Class Checklist.xlsx
+++ b/SlideWinder/Robot Class Checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
   <si>
     <t>Class</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>Robot LEDs</t>
+  </si>
+  <si>
+    <t>Expiremental NetTablesClient</t>
+  </si>
+  <si>
+    <t>don't run customOutputStream</t>
   </si>
 </sst>
 </file>
@@ -238,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -250,6 +256,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -559,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F39"/>
+  <dimension ref="B1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39:F39"/>
+      <selection activeCell="E38" sqref="E38:F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -577,16 +586,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -598,10 +607,10 @@
       <c r="D3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -614,10 +623,10 @@
         <f>IF(EXACT(LOWER(C4), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -630,8 +639,8 @@
         <f t="shared" ref="D5:D35" si="0">IF(EXACT(LOWER(C5), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -644,8 +653,8 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -658,8 +667,8 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -672,10 +681,10 @@
         <f>IF(EXACT(LOWER(C8), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -688,10 +697,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -704,10 +713,10 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
@@ -720,10 +729,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -736,10 +745,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -752,10 +761,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="5"/>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -768,8 +777,8 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
@@ -782,10 +791,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="5"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
@@ -798,10 +807,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="5"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
@@ -814,10 +823,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="5"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
@@ -830,10 +839,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="5"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
@@ -846,10 +855,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="5"/>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
@@ -862,10 +871,10 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
@@ -878,10 +887,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="5"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
@@ -894,10 +903,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F22" s="5"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
@@ -910,10 +919,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F23" s="5"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
@@ -926,10 +935,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="5"/>
+      <c r="F24" s="6"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
@@ -942,10 +951,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F25" s="5"/>
+      <c r="F25" s="6"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
@@ -958,10 +967,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F26" s="5"/>
+      <c r="F26" s="6"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
@@ -974,8 +983,8 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
@@ -988,8 +997,8 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
@@ -1002,10 +1011,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="5"/>
+      <c r="F29" s="6"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
@@ -1018,10 +1027,10 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F30" s="5"/>
+      <c r="F30" s="6"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
@@ -1034,10 +1043,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F31" s="5"/>
+      <c r="F31" s="6"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
@@ -1050,10 +1059,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F32" s="5"/>
+      <c r="F32" s="6"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
@@ -1066,10 +1075,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E33" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F33" s="5"/>
+      <c r="F33" s="6"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
@@ -1082,10 +1091,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F34" s="5"/>
+      <c r="F34" s="6"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
@@ -1098,10 +1107,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F35" s="5"/>
+      <c r="F35" s="6"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
@@ -1114,10 +1123,10 @@
         <f>IF(EXACT(LOWER(C36), "check"), "ü", "û")</f>
         <v>û</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E36" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F36" s="5"/>
+      <c r="F36" s="6"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
@@ -1130,12 +1139,12 @@
         <f>IF(EXACT(LOWER(C37), "check"), "ü", "û")</f>
         <v>û</v>
       </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="1" t="s">
-        <v>51</v>
+      <c r="B38" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>35</v>
@@ -1144,12 +1153,14 @@
         <f>IF(EXACT(LOWER(C38), "check"), "ü", "û")</f>
         <v>û</v>
       </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
+      <c r="E38" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F38" s="6"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>35</v>
@@ -1158,11 +1169,39 @@
         <f>IF(EXACT(LOWER(C39), "check"), "ü", "û")</f>
         <v>û</v>
       </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="E36:F36"/>
@@ -1179,29 +1218,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Elevator and arm now run in the correct direction
Also I updated the offline OI list and the robot checklist.
</commit_message>
<xml_diff>
--- a/SlideWinder/Robot Class Checklist.xlsx
+++ b/SlideWinder/Robot Class Checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="60">
   <si>
     <t>Class</t>
   </si>
@@ -171,9 +171,6 @@
     <t>elevator works, arm untested</t>
   </si>
   <si>
-    <t>Robot Vision</t>
-  </si>
-  <si>
     <t>AutoModeOne_StackTotes</t>
   </si>
   <si>
@@ -189,7 +186,16 @@
     <t>Expiremental NetTablesClient</t>
   </si>
   <si>
-    <t>don't run customOutputStream</t>
+    <t>won' fix</t>
+  </si>
+  <si>
+    <t>might need to be retuned when arm is added</t>
+  </si>
+  <si>
+    <t>AutoVisionFollowLine</t>
+  </si>
+  <si>
+    <t>CameraVision</t>
   </si>
 </sst>
 </file>
@@ -244,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -256,6 +262,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -568,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F40"/>
+  <dimension ref="B1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38:F38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -586,16 +595,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -607,10 +616,10 @@
       <c r="D3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -623,10 +632,10 @@
         <f>IF(EXACT(LOWER(C4), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -636,11 +645,11 @@
         <v>30</v>
       </c>
       <c r="D5" s="2" t="str">
-        <f t="shared" ref="D5:D35" si="0">IF(EXACT(LOWER(C5), "check"), "ü", "û")</f>
+        <f t="shared" ref="D5:D37" si="0">IF(EXACT(LOWER(C5), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -653,12 +662,12 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>30</v>
@@ -667,8 +676,8 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -681,10 +690,10 @@
         <f>IF(EXACT(LOWER(C8), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -697,10 +706,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -713,26 +722,26 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="6"/>
+        <v>ü</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -745,10 +754,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="6"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -761,14 +770,14 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>35</v>
@@ -777,12 +786,12 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>35</v>
@@ -791,10 +800,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="6"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
@@ -807,10 +816,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="6"/>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
@@ -823,78 +832,76 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>û</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E18" s="6" t="s">
+      <c r="C19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>û</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="6"/>
+      <c r="F19" s="7"/>
     </row>
     <row r="20" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D20" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ü</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="6"/>
+        <v>û</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="7"/>
     </row>
     <row r="21" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D21" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="6"/>
+        <v>ü</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="7"/>
     </row>
     <row r="22" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>35</v>
@@ -903,46 +910,46 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="6"/>
+      <c r="E22" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="7"/>
     </row>
     <row r="23" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>û</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E23" s="6" t="s">
+      <c r="C24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>û</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="6"/>
+      <c r="F24" s="7"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>35</v>
@@ -951,14 +958,14 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F25" s="6"/>
+      <c r="E25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="7"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>35</v>
@@ -967,14 +974,14 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F26" s="6"/>
+      <c r="E26" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="7"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>35</v>
@@ -983,74 +990,74 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
+      <c r="E27" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="7"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D28" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ü</v>
-      </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
+        <v>û</v>
+      </c>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D29" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F29" s="6"/>
+        <v>ü</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D30" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ü</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F30" s="6"/>
+        <v>û</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" s="7"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D31" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F31" s="6"/>
+        <v>ü</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" s="7"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>35</v>
@@ -1059,30 +1066,28 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F32" s="6"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" s="1" t="s">
+      <c r="E32" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D33" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F33" s="6"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>35</v>
@@ -1091,14 +1096,14 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E34" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F34" s="6"/>
+      <c r="E34" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" s="7"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>35</v>
@@ -1107,44 +1112,46 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F35" s="6"/>
+      <c r="E35" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" s="7"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D36" s="2" t="str">
-        <f>IF(EXACT(LOWER(C36), "check"), "ü", "û")</f>
-        <v>û</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F36" s="6"/>
+        <f t="shared" si="0"/>
+        <v>û</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F36" s="7"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D37" s="2" t="str">
-        <f>IF(EXACT(LOWER(C37), "check"), "ü", "û")</f>
-        <v>û</v>
-      </c>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
+        <f t="shared" si="0"/>
+        <v>û</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F37" s="7"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="5" t="s">
-        <v>56</v>
+      <c r="B38" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>35</v>
@@ -1153,33 +1160,83 @@
         <f>IF(EXACT(LOWER(C38), "check"), "ü", "û")</f>
         <v>û</v>
       </c>
-      <c r="E38" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F38" s="6"/>
+      <c r="E38" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F38" s="7"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D39" s="2" t="str">
         <f>IF(EXACT(LOWER(C39), "check"), "ü", "û")</f>
-        <v>û</v>
-      </c>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
+        <v>ü</v>
+      </c>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="5" t="s">
         <v>55</v>
       </c>
+      <c r="C40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="2" t="str">
+        <f>IF(EXACT(LOWER(C40), "check"), "ü", "û")</f>
+        <v>û</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" s="2" t="str">
+        <f>IF(EXACT(LOWER(C41), "check"), "ü", "û")</f>
+        <v>û</v>
+      </c>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
+  <mergeCells count="41">
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E39:F39"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E9:F9"/>
@@ -1189,35 +1246,12 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E19:F19"/>
     <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
     <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Removed Elevator Brake from
</commit_message>
<xml_diff>
--- a/SlideWinder/Robot Class Checklist.xlsx
+++ b/SlideWinder/Robot Class Checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="60">
   <si>
     <t>Class</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>worked on test board</t>
+  </si>
+  <si>
+    <t>Immobilize</t>
   </si>
 </sst>
 </file>
@@ -247,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -259,6 +262,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -574,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F41"/>
+  <dimension ref="B1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38:F38"/>
+      <selection activeCell="E17" sqref="E17:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -592,16 +598,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -613,10 +619,10 @@
       <c r="D3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -629,10 +635,10 @@
         <f>IF(EXACT(LOWER(C4), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -642,11 +648,11 @@
         <v>30</v>
       </c>
       <c r="D5" s="2" t="str">
-        <f t="shared" ref="D5:D37" si="0">IF(EXACT(LOWER(C5), "check"), "ü", "û")</f>
-        <v>ü</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+        <f t="shared" ref="D5:D38" si="0">IF(EXACT(LOWER(C5), "check"), "ü", "û")</f>
+        <v>ü</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -659,8 +665,8 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -673,8 +679,8 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -687,10 +693,10 @@
         <f>IF(EXACT(LOWER(C8), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -703,10 +709,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -719,10 +725,10 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
@@ -735,10 +741,10 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="7"/>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -751,8 +757,8 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -765,10 +771,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -781,8 +787,8 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
@@ -795,10 +801,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="8"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
@@ -811,26 +817,24 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="8"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="7"/>
+        <v>ü</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
@@ -843,8 +847,8 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
@@ -857,10 +861,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="7"/>
+      <c r="F19" s="8"/>
     </row>
     <row r="20" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
@@ -873,10 +877,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="7"/>
+      <c r="F20" s="8"/>
     </row>
     <row r="21" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
@@ -889,10 +893,10 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="7"/>
+      <c r="F21" s="8"/>
     </row>
     <row r="22" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
@@ -905,62 +909,60 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="7"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
     </row>
     <row r="24" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>û</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E24" s="7" t="s">
+      <c r="C25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>û</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="7"/>
+      <c r="F25" s="8"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>35</v>
@@ -969,14 +971,14 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F26" s="7"/>
+      <c r="E26" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" s="8"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>35</v>
@@ -985,14 +987,14 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F27" s="7"/>
+      <c r="E27" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="8"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>35</v>
@@ -1001,26 +1003,28 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="E28" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" s="8"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D29" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ü</v>
-      </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+        <v>û</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>30</v>
@@ -1029,12 +1033,12 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>30</v>
@@ -1043,60 +1047,58 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" s="7"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>ü</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="8"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D32" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E32" s="7" t="s">
+      <c r="C33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>û</v>
+      </c>
+      <c r="E33" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="6" t="s">
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D34" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E34" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F34" s="7"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>35</v>
@@ -1105,14 +1107,14 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E35" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F35" s="7"/>
+      <c r="E35" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" s="8"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>35</v>
@@ -1121,14 +1123,14 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E36" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F36" s="7"/>
+      <c r="E36" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36" s="8"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>35</v>
@@ -1137,30 +1139,30 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E37" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F37" s="7"/>
+      <c r="E37" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F37" s="8"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D38" s="2" t="str">
-        <f>IF(EXACT(LOWER(C38), "check"), "ü", "û")</f>
-        <v>ü</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F38" s="7"/>
+        <f t="shared" si="0"/>
+        <v>û</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" s="8"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>30</v>
@@ -1169,28 +1171,28 @@
         <f>IF(EXACT(LOWER(C39), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
+      <c r="E39" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" s="8"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="5" t="s">
-        <v>53</v>
+      <c r="B40" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D40" s="2" t="str">
         <f>IF(EXACT(LOWER(C40), "check"), "ü", "û")</f>
-        <v>û</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F40" s="7"/>
+        <v>ü</v>
+      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
-        <v>52</v>
+      <c r="B41" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>35</v>
@@ -1199,52 +1201,69 @@
         <f>IF(EXACT(LOWER(C41), "check"), "ü", "û")</f>
         <v>û</v>
       </c>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
+      <c r="E41" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F41" s="8"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" s="2" t="str">
+        <f>IF(EXACT(LOWER(C42), "check"), "ü", "û")</f>
+        <v>û</v>
+      </c>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+  <mergeCells count="42">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E24:F24"/>
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E23:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Removed Elevator Brake from"
This reverts commit 80d838a055dbc837a4b89749507192eb582f811d.
</commit_message>
<xml_diff>
--- a/SlideWinder/Robot Class Checklist.xlsx
+++ b/SlideWinder/Robot Class Checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
   <si>
     <t>Class</t>
   </si>
@@ -193,9 +193,6 @@
   </si>
   <si>
     <t>worked on test board</t>
-  </si>
-  <si>
-    <t>Immobilize</t>
   </si>
 </sst>
 </file>
@@ -250,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -262,9 +259,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -580,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F42"/>
+  <dimension ref="B1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:F17"/>
+      <selection activeCell="E38" sqref="E38:F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -598,16 +592,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -619,10 +613,10 @@
       <c r="D3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="9"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -635,10 +629,10 @@
         <f>IF(EXACT(LOWER(C4), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -648,11 +642,11 @@
         <v>30</v>
       </c>
       <c r="D5" s="2" t="str">
-        <f t="shared" ref="D5:D38" si="0">IF(EXACT(LOWER(C5), "check"), "ü", "û")</f>
+        <f t="shared" ref="D5:D37" si="0">IF(EXACT(LOWER(C5), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -665,8 +659,8 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -679,8 +673,8 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -693,10 +687,10 @@
         <f>IF(EXACT(LOWER(C8), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -709,10 +703,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -725,10 +719,10 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
@@ -741,10 +735,10 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -757,8 +751,8 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -771,10 +765,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -787,8 +781,8 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
@@ -801,10 +795,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="8"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
@@ -817,24 +811,26 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ü</v>
-      </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+        <v>û</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="7"/>
     </row>
     <row r="18" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
@@ -847,8 +843,8 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
@@ -861,10 +857,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="8"/>
+      <c r="F19" s="7"/>
     </row>
     <row r="20" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
@@ -877,10 +873,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="8"/>
+      <c r="F20" s="7"/>
     </row>
     <row r="21" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
@@ -893,10 +889,10 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="8"/>
+      <c r="F21" s="7"/>
     </row>
     <row r="22" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
@@ -909,28 +905,30 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="7" t="s">
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
+      <c r="E23" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="7"/>
     </row>
     <row r="24" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>35</v>
@@ -939,30 +937,30 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E24" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="E24" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D25" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E25" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F25" s="8"/>
+      <c r="E25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="7"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>35</v>
@@ -971,14 +969,14 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E26" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F26" s="8"/>
+      <c r="E26" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="7"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>35</v>
@@ -987,14 +985,14 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E27" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27" s="8"/>
+      <c r="E27" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="7"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>35</v>
@@ -1003,28 +1001,26 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E28" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F28" s="8"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D29" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
+        <v>ü</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>30</v>
@@ -1033,12 +1029,12 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>30</v>
@@ -1047,58 +1043,60 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
+      <c r="E31" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="7"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D32" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ü</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F32" s="8"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="1" t="s">
+        <v>û</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D33" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E33" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F33" s="8"/>
-    </row>
-    <row r="34" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="6" t="s">
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D34" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
+      <c r="E34" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" s="7"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>35</v>
@@ -1107,14 +1105,14 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E35" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F35" s="8"/>
+      <c r="E35" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F35" s="7"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>35</v>
@@ -1123,14 +1121,14 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E36" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F36" s="8"/>
+      <c r="E36" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F36" s="7"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>35</v>
@@ -1139,30 +1137,30 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E37" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F37" s="8"/>
+      <c r="E37" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F37" s="7"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D38" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F38" s="8"/>
+        <f>IF(EXACT(LOWER(C38), "check"), "ü", "û")</f>
+        <v>ü</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F38" s="7"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>30</v>
@@ -1171,28 +1169,28 @@
         <f>IF(EXACT(LOWER(C39), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
-      <c r="E39" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F39" s="8"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
-        <v>42</v>
+      <c r="B40" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D40" s="2" t="str">
         <f>IF(EXACT(LOWER(C40), "check"), "ü", "û")</f>
-        <v>ü</v>
-      </c>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
+        <v>û</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F40" s="7"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="5" t="s">
-        <v>53</v>
+      <c r="B41" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>35</v>
@@ -1201,69 +1199,52 @@
         <f>IF(EXACT(LOWER(C41), "check"), "ü", "û")</f>
         <v>û</v>
       </c>
-      <c r="E41" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F41" s="8"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D42" s="2" t="str">
-        <f>IF(EXACT(LOWER(C42), "check"), "ü", "û")</f>
-        <v>û</v>
-      </c>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
+  <mergeCells count="41">
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E31:F31"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E28:F28"/>
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E23:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Put DeployPiston in the correct position & removed ElevatorBrake
The robot now uses only one PCM. The checklist has been updated with the
immoblize command.
</commit_message>
<xml_diff>
--- a/SlideWinder/Robot Class Checklist.xlsx
+++ b/SlideWinder/Robot Class Checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="60">
   <si>
     <t>Class</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>worked on test board</t>
+  </si>
+  <si>
+    <t>Immobilize</t>
   </si>
 </sst>
 </file>
@@ -247,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -259,6 +262,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -574,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F41"/>
+  <dimension ref="B1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38:F38"/>
+      <selection activeCell="E23" sqref="E23:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -592,16 +598,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -613,10 +619,10 @@
       <c r="D3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -629,10 +635,10 @@
         <f>IF(EXACT(LOWER(C4), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -642,11 +648,11 @@
         <v>30</v>
       </c>
       <c r="D5" s="2" t="str">
-        <f t="shared" ref="D5:D37" si="0">IF(EXACT(LOWER(C5), "check"), "ü", "û")</f>
+        <f t="shared" ref="D5:D38" si="0">IF(EXACT(LOWER(C5), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -659,8 +665,8 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -673,8 +679,8 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -687,10 +693,10 @@
         <f>IF(EXACT(LOWER(C8), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -703,10 +709,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -719,10 +725,10 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
@@ -735,10 +741,10 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="7"/>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -751,8 +757,8 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -765,10 +771,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -781,8 +787,8 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
@@ -795,10 +801,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="8"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
@@ -811,10 +817,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="8"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
@@ -827,10 +833,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="7"/>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
@@ -843,8 +849,8 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
@@ -857,10 +863,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="7"/>
+      <c r="F19" s="8"/>
     </row>
     <row r="20" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
@@ -873,10 +879,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="7"/>
+      <c r="F20" s="8"/>
     </row>
     <row r="21" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
@@ -889,10 +895,10 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="7"/>
+      <c r="F21" s="8"/>
     </row>
     <row r="22" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
@@ -905,62 +911,60 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="7"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
     </row>
     <row r="24" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>û</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E24" s="7" t="s">
+      <c r="C25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>û</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="7"/>
+      <c r="F25" s="8"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>35</v>
@@ -969,14 +973,14 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F26" s="7"/>
+      <c r="E26" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" s="8"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>35</v>
@@ -985,14 +989,14 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F27" s="7"/>
+      <c r="E27" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="8"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>35</v>
@@ -1001,26 +1005,28 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="E28" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" s="8"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D29" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ü</v>
-      </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+        <v>û</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>30</v>
@@ -1029,12 +1035,12 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>30</v>
@@ -1043,60 +1049,58 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" s="7"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>ü</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="8"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D32" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E32" s="7" t="s">
+      <c r="C33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>û</v>
+      </c>
+      <c r="E33" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="6" t="s">
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D34" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E34" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F34" s="7"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>35</v>
@@ -1105,14 +1109,14 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E35" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F35" s="7"/>
+      <c r="E35" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" s="8"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>35</v>
@@ -1121,14 +1125,14 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E36" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F36" s="7"/>
+      <c r="E36" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36" s="8"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>35</v>
@@ -1137,30 +1141,30 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E37" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F37" s="7"/>
+      <c r="E37" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F37" s="8"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D38" s="2" t="str">
-        <f>IF(EXACT(LOWER(C38), "check"), "ü", "û")</f>
-        <v>ü</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F38" s="7"/>
+        <f t="shared" si="0"/>
+        <v>û</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" s="8"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>30</v>
@@ -1169,28 +1173,28 @@
         <f>IF(EXACT(LOWER(C39), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
+      <c r="E39" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" s="8"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="5" t="s">
-        <v>53</v>
+      <c r="B40" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D40" s="2" t="str">
         <f>IF(EXACT(LOWER(C40), "check"), "ü", "û")</f>
-        <v>û</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F40" s="7"/>
+        <v>ü</v>
+      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
-        <v>52</v>
+      <c r="B41" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>35</v>
@@ -1199,52 +1203,69 @@
         <f>IF(EXACT(LOWER(C41), "check"), "ü", "û")</f>
         <v>û</v>
       </c>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
+      <c r="E41" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F41" s="8"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" s="2" t="str">
+        <f>IF(EXACT(LOWER(C42), "check"), "ü", "û")</f>
+        <v>û</v>
+      </c>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+  <mergeCells count="42">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E24:F24"/>
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E23:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
CloseClaw, Open Claw, and AutoCalibrateElevator are checked off
Also the elevator PID is tuned and SetElevatorPosition is ready to be
tested.
</commit_message>
<xml_diff>
--- a/SlideWinder/Robot Class Checklist.xlsx
+++ b/SlideWinder/Robot Class Checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="62">
   <si>
     <t>Class</t>
   </si>
@@ -126,9 +126,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>needs limit switches and tuning</t>
-  </si>
-  <si>
     <t>Deploy Arm</t>
   </si>
   <si>
@@ -193,6 +190,18 @@
   </si>
   <si>
     <t>worked on test board</t>
+  </si>
+  <si>
+    <t>Immobilize</t>
+  </si>
+  <si>
+    <t>QuickStackOne</t>
+  </si>
+  <si>
+    <t>QuickStackTwo</t>
+  </si>
+  <si>
+    <t>PID is tuned</t>
   </si>
 </sst>
 </file>
@@ -247,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -259,6 +268,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -574,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F41"/>
+  <dimension ref="B1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38:F38"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -592,16 +607,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -613,10 +628,10 @@
       <c r="D3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="10"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -629,10 +644,10 @@
         <f>IF(EXACT(LOWER(C4), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="7"/>
+      <c r="E4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="9"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -642,11 +657,11 @@
         <v>30</v>
       </c>
       <c r="D5" s="2" t="str">
-        <f t="shared" ref="D5:D37" si="0">IF(EXACT(LOWER(C5), "check"), "ü", "û")</f>
-        <v>ü</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+        <f t="shared" ref="D5:D40" si="0">IF(EXACT(LOWER(C5), "check"), "ü", "û")</f>
+        <v>ü</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -659,12 +674,12 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>30</v>
@@ -673,8 +688,8 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -687,26 +702,24 @@
         <f>IF(EXACT(LOWER(C8), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="7"/>
+      <c r="E8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="7"/>
+        <v>ü</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -719,10 +732,10 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="7"/>
+      <c r="E10" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="9"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
@@ -735,10 +748,10 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="7"/>
+      <c r="E11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -751,8 +764,8 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -765,14 +778,14 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="9"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>35</v>
@@ -781,12 +794,12 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>35</v>
@@ -795,10 +808,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
@@ -811,10 +824,10 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="9"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
@@ -827,14 +840,14 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="7"/>
+      <c r="F17" s="9"/>
     </row>
     <row r="18" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>35</v>
@@ -843,28 +856,26 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D19" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="7"/>
+        <v>ü</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>35</v>
@@ -873,14 +884,14 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="7"/>
+      <c r="F20" s="9"/>
     </row>
     <row r="21" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>30</v>
@@ -889,14 +900,14 @@
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" s="7"/>
+      <c r="E21" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="9"/>
     </row>
     <row r="22" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>35</v>
@@ -905,30 +916,28 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="E22" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="7"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>35</v>
@@ -937,62 +946,56 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>35</v>
+      <c r="E24" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="D25" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="7"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="1" t="s">
+        <v>ü</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="2:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>35</v>
       </c>
       <c r="D26" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="2:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>35</v>
       </c>
       <c r="D27" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F27" s="7"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>35</v>
@@ -1001,102 +1004,104 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="E28" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="9"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D29" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ü</v>
-      </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+        <v>û</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" s="9"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D30" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ü</v>
-      </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+        <v>û</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" s="9"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D31" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ü</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" s="7"/>
+        <v>û</v>
+      </c>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D32" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>35</v>
+        <v>ü</v>
+      </c>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="D33" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+        <v>ü</v>
+      </c>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D34" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F34" s="7"/>
+        <v>ü</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" s="9"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>35</v>
@@ -1105,30 +1110,28 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E35" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F35" s="7"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="E35" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D36" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E36" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F36" s="7"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>35</v>
@@ -1137,90 +1140,154 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E37" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F37" s="7"/>
+      <c r="E37" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" s="9"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D38" s="2" t="str">
-        <f>IF(EXACT(LOWER(C38), "check"), "ü", "û")</f>
-        <v>ü</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F38" s="7"/>
+        <f t="shared" si="0"/>
+        <v>û</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" s="9"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D39" s="2" t="str">
-        <f>IF(EXACT(LOWER(C39), "check"), "ü", "û")</f>
-        <v>ü</v>
-      </c>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
+        <f t="shared" si="0"/>
+        <v>û</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" s="9"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="5" t="s">
-        <v>53</v>
+      <c r="B40" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D40" s="2" t="str">
-        <f>IF(EXACT(LOWER(C40), "check"), "ü", "û")</f>
-        <v>û</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F40" s="7"/>
+        <f t="shared" si="0"/>
+        <v>û</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F40" s="9"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D41" s="2" t="str">
         <f>IF(EXACT(LOWER(C41), "check"), "ü", "û")</f>
-        <v>û</v>
-      </c>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
+        <v>ü</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F41" s="9"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="2" t="str">
+        <f>IF(EXACT(LOWER(C42), "check"), "ü", "û")</f>
+        <v>ü</v>
+      </c>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" s="2" t="str">
+        <f>IF(EXACT(LOWER(C43), "check"), "ü", "û")</f>
+        <v>û</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F43" s="9"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="2" t="str">
+        <f>IF(EXACT(LOWER(C44), "check"), "ü", "û")</f>
+        <v>û</v>
+      </c>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="E39:F39"/>
+  <mergeCells count="44">
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E42:F42"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E43:F43"/>
     <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
     <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E9:F9"/>
@@ -1232,19 +1299,6 @@
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>